<commit_message>
handle order admin and checkout payment
</commit_message>
<xml_diff>
--- a/storage/reservations.xlsx
+++ b/storage/reservations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -99,6 +99,63 @@
   </si>
   <si>
     <t>CHO_DUYET</t>
+  </si>
+  <si>
+    <t>Vy</t>
+  </si>
+  <si>
+    <t>0534243296</t>
+  </si>
+  <si>
+    <t>2026-01-08</t>
+  </si>
+  <si>
+    <t>16:45</t>
+  </si>
+  <si>
+    <t>okela</t>
+  </si>
+  <si>
+    <t>0541223212</t>
+  </si>
+  <si>
+    <t>16:56</t>
+  </si>
+  <si>
+    <t>View thoáng mát nha</t>
+  </si>
+  <si>
+    <t>0869803823</t>
+  </si>
+  <si>
+    <t>Trong nhà nhé</t>
+  </si>
+  <si>
+    <t>Trung</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>2026-01-09</t>
+  </si>
+  <si>
+    <t>16:58</t>
+  </si>
+  <si>
+    <t>Xanh sạch đẹp</t>
+  </si>
+  <si>
+    <t>0543432412</t>
+  </si>
+  <si>
+    <t>2026-01-06</t>
+  </si>
+  <si>
+    <t>20:07</t>
+  </si>
+  <si>
+    <t>Tầng 2 thì càng tốt</t>
   </si>
 </sst>
 </file>
@@ -438,13 +495,22 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="9" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="2" max="2" width="15.363636363636" customWidth="true" style="0"/>
+    <col min="3" max="3" width="15.818181818182" customWidth="true" style="0"/>
+    <col min="4" max="4" width="8.8181818181818" customWidth="true" style="0"/>
+    <col min="5" max="5" width="11" customWidth="true" style="0"/>
+    <col min="6" max="6" width="6.0909090909091" customWidth="true" style="0"/>
+    <col min="7" max="7" width="20.363636363636" customWidth="true" style="0"/>
+    <col min="8" max="8" width="12.090909090909" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -573,10 +639,140 @@
         <v>27</v>
       </c>
     </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>